<commit_message>
OPERA Report - WIP in calc vat and service charge
</commit_message>
<xml_diff>
--- a/Saudi/Cancel Booking.xlsx
+++ b/Saudi/Cancel Booking.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Booking No</t>
   </si>
@@ -27,21 +27,15 @@
     <t>Cancel Reason</t>
   </si>
   <si>
-    <t>Chargable Days</t>
+    <t>Chargeable Days</t>
   </si>
   <si>
     <t>Daily Rate</t>
   </si>
   <si>
-    <t>Total Rate</t>
-  </si>
-  <si>
     <t>Discount Amount</t>
   </si>
   <si>
-    <t>Room Tax</t>
-  </si>
-  <si>
     <t>Pay Method</t>
   </si>
   <si>
@@ -57,10 +51,31 @@
     <t>Cancel Date</t>
   </si>
   <si>
+    <t>Rate Code</t>
+  </si>
+  <si>
+    <t>CXL</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>OARRO</t>
+  </si>
+  <si>
     <t>PLC</t>
   </si>
   <si>
-    <t>CL</t>
+    <t>ANEXBB</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>OST3HB</t>
+  </si>
+  <si>
+    <t>RACK</t>
   </si>
 </sst>
 </file>
@@ -203,8 +218,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="6"/>
-      <color rgb="FF000000"/>
+      <sz val="7"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -565,10 +580,10 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="4" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="15" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -895,29 +910,27 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="1" customWidth="1"/>
-    <col min="9" max="10" width="13.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -951,44 +964,139 @@
       <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>77901</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>18406</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3">
+        <v>500.01</v>
+      </c>
+      <c r="E2" s="3">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>289.27999999999997</v>
-      </c>
-      <c r="E2" s="4">
-        <v>2314.2399999999998</v>
-      </c>
-      <c r="F2" s="2"/>
       <c r="G2" s="3">
         <v>0</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4">
+        <v>43548</v>
+      </c>
+      <c r="I2" s="4">
+        <v>43556</v>
+      </c>
+      <c r="J2" s="4">
+        <v>43548</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="3">
+    </row>
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>18406</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3">
+        <v>289.27999999999997</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="3">
         <v>0</v>
       </c>
-      <c r="J2" s="5">
+      <c r="H3" s="4">
         <v>43550</v>
       </c>
-      <c r="K2" s="5">
+      <c r="I3" s="4">
         <v>43558</v>
       </c>
-      <c r="L2" s="5">
+      <c r="J3" s="4">
         <v>43548</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>24652</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3">
+        <v>722</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>43586</v>
+      </c>
+      <c r="I4" s="4">
+        <v>43590</v>
+      </c>
+      <c r="J4" s="4">
+        <v>43548</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>77655</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>43548</v>
+      </c>
+      <c r="I5" s="4">
+        <v>43553</v>
+      </c>
+      <c r="J5" s="4">
+        <v>43548</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OPERA Report - WIP in calc grand total
</commit_message>
<xml_diff>
--- a/Saudi/Cancel Booking.xlsx
+++ b/Saudi/Cancel Booking.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Booking No</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>Chargeable Days</t>
+  </si>
+  <si>
+    <t>No. of Rooms</t>
   </si>
   <si>
     <t>Daily Rate</t>
@@ -910,27 +913,30 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E2:E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -964,139 +970,154 @@
       <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>77901</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3">
         <v>8</v>
       </c>
       <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3">
         <v>500.01</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="3">
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="3">
         <v>0</v>
       </c>
-      <c r="H2" s="4">
+      <c r="I2" s="4">
         <v>43548</v>
       </c>
-      <c r="I2" s="4">
+      <c r="J2" s="4">
         <v>43556</v>
       </c>
-      <c r="J2" s="4">
+      <c r="K2" s="4">
         <v>43548</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>13</v>
+      <c r="L2" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>18406</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3">
         <v>8</v>
       </c>
       <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
         <v>289.27999999999997</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="F3" s="2"/>
+      <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="3">
         <v>0</v>
       </c>
-      <c r="H3" s="4">
+      <c r="I3" s="4">
         <v>43550</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="4">
         <v>43558</v>
       </c>
-      <c r="J3" s="4">
+      <c r="K3" s="4">
         <v>43548</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>15</v>
+      <c r="L3" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>24652</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3">
         <v>4</v>
       </c>
       <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
         <v>722</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="F4" s="2"/>
+      <c r="G4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="3">
         <v>0</v>
       </c>
-      <c r="H4" s="4">
+      <c r="I4" s="4">
         <v>43586</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="4">
         <v>43590</v>
       </c>
-      <c r="J4" s="4">
+      <c r="K4" s="4">
         <v>43548</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>17</v>
+      <c r="L4" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>77655</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3">
         <v>5</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
         <v>2500</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="F5" s="2"/>
+      <c r="G5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="3">
         <v>0</v>
       </c>
-      <c r="H5" s="4">
+      <c r="I5" s="4">
         <v>43548</v>
       </c>
-      <c r="I5" s="4">
+      <c r="J5" s="4">
         <v>43553</v>
       </c>
-      <c r="J5" s="4">
+      <c r="K5" s="4">
         <v>43548</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>18</v>
+      <c r="L5" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>